<commit_message>
Lagt till åtgärd i backlog
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maja\Desktop\ProjectPetra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Desktop\ProjectPetra\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="101">
   <si>
     <t>Snabb översikt över produktionen</t>
   </si>
@@ -323,6 +323,12 @@
   </si>
   <si>
     <t>Logga ut funktion</t>
+  </si>
+  <si>
+    <t>RoleAdmin/admin tabeller</t>
+  </si>
+  <si>
+    <t>Tabellerna måste göras responsiva</t>
   </si>
 </sst>
 </file>
@@ -1217,7 +1223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1963,9 +1969,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -2020,6 +2026,17 @@
         <v>56</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Lagt till item i backlog
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="103">
   <si>
     <t>Snabb översikt över produktionen</t>
   </si>
@@ -329,6 +329,12 @@
   </si>
   <si>
     <t>Tabellerna måste göras responsiva</t>
+  </si>
+  <si>
+    <t>Säkra upp web api:erna</t>
+  </si>
+  <si>
+    <t>Läggas Authorize attribut på api:erna</t>
   </si>
 </sst>
 </file>
@@ -1969,10 +1975,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2037,6 +2043,17 @@
         <v>100</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Change for layout and Backlog
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Desktop\ProjectPetra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maja\Desktop\ProjectPetra\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1247,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="E12" s="68"/>
       <c r="F12" s="53" t="s">
-        <v>108</v>
+        <v>48</v>
       </c>
       <c r="G12" s="73" t="s">
         <v>91</v>
@@ -1475,8 +1475,8 @@
         <v>8</v>
       </c>
       <c r="E13" s="68"/>
-      <c r="F13" s="68" t="s">
-        <v>57</v>
+      <c r="F13" s="53" t="s">
+        <v>48</v>
       </c>
       <c r="G13" s="73" t="s">
         <v>97</v>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="E14" s="68"/>
       <c r="F14" s="53" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="G14" s="73" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
Added Deadline in edit from
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="113">
   <si>
     <t>Snabb översikt över produktionen</t>
   </si>
@@ -134,9 +134,6 @@
   </si>
   <si>
     <t>Se planering för 1-2mån framåt</t>
-  </si>
-  <si>
-    <t>Backlog items</t>
   </si>
   <si>
     <t>Item number</t>
@@ -374,7 +371,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,14 +407,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -558,7 +547,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -636,43 +625,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -759,9 +711,9 @@
     <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
@@ -785,7 +737,6 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="5" xfId="11" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="4" applyBorder="1"/>
@@ -799,48 +750,35 @@
     <xf numFmtId="0" fontId="4" fillId="17" borderId="7" xfId="11" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="8" xfId="13" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="13" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="8" xfId="12" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="8" xfId="12" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="8" xfId="15" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" xfId="14" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="10" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="8" xfId="16" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="9" xfId="16" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="8" xfId="15" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="8" xfId="14" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="10" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="8" xfId="16" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="9" xfId="16" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="10" xfId="11" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="11" xfId="13" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="12" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="8" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="11" xfId="15" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="6" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="11" xfId="14" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="10" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="11" xfId="16" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="12" xfId="16" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="11" xfId="15" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="11" xfId="14" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="11" xfId="16" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="12" xfId="16" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="11" xfId="13" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="11" xfId="12" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="8" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="10" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="8" xfId="13" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="8" xfId="12" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="8" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="10" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="6" xfId="12" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="13" xfId="16" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="10" xfId="16" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="6" xfId="16" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="6" xfId="14" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="15" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="14" xfId="17" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="14" xfId="11" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="11" xfId="17" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="11" xfId="11" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="20% - Dekorfärg1" xfId="12" builtinId="30"/>
@@ -866,6 +804,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9966"/>
       <color rgb="FFB17ED8"/>
       <color rgb="FFFDBCB1"/>
       <color rgb="FFFF5D5D"/>
@@ -1282,558 +1221,524 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A2:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="83.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="83.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="E3" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="34">
+        <v>1</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="34">
+        <v>16</v>
+      </c>
+      <c r="D4" s="34">
+        <v>1</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="34">
+        <v>2</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="34">
+        <v>32</v>
+      </c>
+      <c r="D5" s="34">
+        <v>1</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="34">
+        <v>3</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="34">
+        <v>16</v>
+      </c>
+      <c r="D6" s="34">
+        <v>1</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="35">
+        <v>4</v>
+      </c>
+      <c r="B7" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="48">
-        <v>1</v>
-      </c>
-      <c r="C4" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="48">
+      <c r="C7" s="35">
         <v>16</v>
       </c>
-      <c r="E4" s="48">
-        <v>1</v>
-      </c>
-      <c r="F4" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
-      <c r="B5" s="48">
+      <c r="D7" s="35"/>
+      <c r="E7" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="25"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="52">
+        <v>5</v>
+      </c>
+      <c r="D8" s="52"/>
+      <c r="E8" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="52">
+        <v>5</v>
+      </c>
+      <c r="D9" s="52"/>
+      <c r="E9" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="52">
+        <v>6</v>
+      </c>
+      <c r="D10" s="52"/>
+      <c r="E10" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="37">
+        <v>5</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="37">
+        <v>56</v>
+      </c>
+      <c r="D11" s="37"/>
+      <c r="E11" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="57"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="53">
+        <v>16</v>
+      </c>
+      <c r="D12" s="53"/>
+      <c r="E12" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="58" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="53">
+        <v>8</v>
+      </c>
+      <c r="D13" s="53"/>
+      <c r="E13" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="58" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="53">
+        <v>16</v>
+      </c>
+      <c r="D14" s="53"/>
+      <c r="E14" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="58" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="53">
+        <v>16</v>
+      </c>
+      <c r="D15" s="53"/>
+      <c r="E15" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="58" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="39">
+        <v>6</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="39">
+        <v>22</v>
+      </c>
+      <c r="D16" s="39"/>
+      <c r="E16" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="27"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="48">
+        <v>4</v>
+      </c>
+      <c r="D17" s="48"/>
+      <c r="E17" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="48">
         <v>2</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="48">
-        <v>32</v>
-      </c>
-      <c r="E5" s="48">
-        <v>1</v>
-      </c>
-      <c r="F5" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="48">
-        <v>3</v>
-      </c>
-      <c r="C6" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="48">
-        <v>16</v>
-      </c>
-      <c r="E6" s="48">
-        <v>1</v>
-      </c>
-      <c r="F6" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="25" t="s">
+      <c r="D18" s="48"/>
+      <c r="E18" s="40" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="49">
+      <c r="F18" s="62" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="48">
+        <v>8</v>
+      </c>
+      <c r="D19" s="48"/>
+      <c r="E19" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="48">
+        <v>8</v>
+      </c>
+      <c r="D20" s="48"/>
+      <c r="E20" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="41">
+        <v>7</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="41">
+        <v>22</v>
+      </c>
+      <c r="D21" s="41"/>
+      <c r="E21" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21" s="29"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="49">
         <v>4</v>
       </c>
-      <c r="C7" s="60" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="49">
-        <v>16</v>
-      </c>
-      <c r="E7" s="49"/>
-      <c r="F7" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" s="26"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="66">
-        <v>5</v>
-      </c>
-      <c r="E8" s="66"/>
-      <c r="F8" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="66">
-        <v>5</v>
-      </c>
-      <c r="E9" s="66"/>
-      <c r="F9" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="50" t="s">
-        <v>98</v>
-      </c>
-      <c r="D10" s="66">
-        <v>6</v>
-      </c>
-      <c r="E10" s="66"/>
-      <c r="F10" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="51">
-        <v>5</v>
-      </c>
-      <c r="C11" s="61" t="s">
+      <c r="D22" s="49"/>
+      <c r="E22" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="49">
+        <v>2</v>
+      </c>
+      <c r="D23" s="49"/>
+      <c r="E23" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="61" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="49">
+        <v>8</v>
+      </c>
+      <c r="D24" s="49"/>
+      <c r="E24" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="49">
+        <v>8</v>
+      </c>
+      <c r="D25" s="49"/>
+      <c r="E25" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" s="30" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="43">
+        <v>8</v>
+      </c>
+      <c r="B26" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="43">
+        <v>26</v>
+      </c>
+      <c r="D26" s="43"/>
+      <c r="E26" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="31"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="51">
+      <c r="C27" s="50">
+        <v>8</v>
+      </c>
+      <c r="D27" s="50"/>
+      <c r="E27" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="51"/>
-      <c r="F11" s="61" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="71"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="52" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="52" t="s">
+      <c r="F27" s="32" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="67">
-        <v>16</v>
-      </c>
-      <c r="E12" s="67"/>
-      <c r="F12" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="72" t="s">
+      <c r="C28" s="50">
+        <v>2</v>
+      </c>
+      <c r="D28" s="50"/>
+      <c r="E28" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="60" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="50">
+        <v>8</v>
+      </c>
+      <c r="D29" s="50"/>
+      <c r="E29" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="32" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="67">
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="51">
         <v>8</v>
       </c>
-      <c r="E13" s="67"/>
-      <c r="F13" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="72" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="67">
-        <v>16</v>
-      </c>
-      <c r="E14" s="67"/>
-      <c r="F14" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="72" t="s">
+      <c r="D30" s="51"/>
+      <c r="E30" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="59" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="52" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="67">
-        <v>16</v>
-      </c>
-      <c r="E15" s="67"/>
-      <c r="F15" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="72" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="53">
-        <v>6</v>
-      </c>
-      <c r="C16" s="53" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="53">
-        <v>22</v>
-      </c>
-      <c r="E16" s="53"/>
-      <c r="F16" s="68" t="s">
-        <v>106</v>
-      </c>
-      <c r="G16" s="28"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="54" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="62">
-        <v>4</v>
-      </c>
-      <c r="E17" s="62"/>
-      <c r="F17" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="62" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="62">
-        <v>2</v>
-      </c>
-      <c r="E18" s="62"/>
-      <c r="F18" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="G18" s="76" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="54" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="62">
-        <v>8</v>
-      </c>
-      <c r="E19" s="62"/>
-      <c r="F19" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
-      <c r="B20" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" s="62" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="62">
-        <v>8</v>
-      </c>
-      <c r="E20" s="62"/>
-      <c r="F20" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="G20" s="29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
-      <c r="B21" s="55">
-        <v>7</v>
-      </c>
-      <c r="C21" s="55" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="55">
-        <v>22</v>
-      </c>
-      <c r="E21" s="55"/>
-      <c r="F21" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="G21" s="30"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
-      <c r="B22" s="56" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="63" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="63">
-        <v>4</v>
-      </c>
-      <c r="E22" s="63"/>
-      <c r="F22" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" s="31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
-      <c r="B23" s="56" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="63">
-        <v>2</v>
-      </c>
-      <c r="E23" s="63"/>
-      <c r="F23" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="G23" s="75" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
-      <c r="B24" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="63">
-        <v>8</v>
-      </c>
-      <c r="E24" s="63"/>
-      <c r="F24" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="G24" s="31" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="43"/>
-      <c r="B25" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="63">
-        <v>8</v>
-      </c>
-      <c r="E25" s="63"/>
-      <c r="F25" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="G25" s="31" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
-      <c r="B26" s="57">
-        <v>8</v>
-      </c>
-      <c r="C26" s="57" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="57">
-        <v>26</v>
-      </c>
-      <c r="E26" s="57"/>
-      <c r="F26" s="70" t="s">
-        <v>57</v>
-      </c>
-      <c r="G26" s="32"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="45"/>
-      <c r="B27" s="58" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" s="64" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="64">
-        <v>8</v>
-      </c>
-      <c r="E27" s="64"/>
-      <c r="F27" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="G27" s="33" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="45"/>
-      <c r="B28" s="58" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28" s="64" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28" s="64">
-        <v>2</v>
-      </c>
-      <c r="E28" s="64"/>
-      <c r="F28" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="G28" s="74" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="45"/>
-      <c r="B29" s="58" t="s">
-        <v>89</v>
-      </c>
-      <c r="C29" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="D29" s="64">
-        <v>8</v>
-      </c>
-      <c r="E29" s="64"/>
-      <c r="F29" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="G29" s="33" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="46"/>
-      <c r="B30" s="59" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="65" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" s="65">
-        <v>8</v>
-      </c>
-      <c r="E30" s="65"/>
-      <c r="F30" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="G30" s="73" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2032,7 +1937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -2044,138 +1949,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="63"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="63">
+        <v>1</v>
+      </c>
+      <c r="B2" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="77" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="77" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="77"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="77">
-        <v>1</v>
-      </c>
-      <c r="B2" s="77" t="s">
+      <c r="C2" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="D2" s="63"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="64">
+        <v>2</v>
+      </c>
+      <c r="B3" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="77"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="78">
-        <v>2</v>
-      </c>
-      <c r="B3" s="78" t="s">
+      <c r="C3" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="D3" s="64" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="63">
+        <v>3</v>
+      </c>
+      <c r="B4" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="C4" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="63"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="63">
+        <v>4</v>
+      </c>
+      <c r="B5" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="63"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="63">
+        <v>5</v>
+      </c>
+      <c r="B6" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="63" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="77">
-        <v>3</v>
-      </c>
-      <c r="B4" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="77" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="77"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="77">
-        <v>4</v>
-      </c>
-      <c r="B5" s="77" t="s">
-        <v>99</v>
-      </c>
-      <c r="C5" s="77" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="77"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="77">
-        <v>5</v>
-      </c>
-      <c r="B6" s="77" t="s">
+      <c r="D6" s="63"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="63">
+        <v>6</v>
+      </c>
+      <c r="B7" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="77" t="s">
+      <c r="C7" s="63" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" s="63"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="63">
+        <v>7</v>
+      </c>
+      <c r="B8" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="63">
+        <v>8</v>
+      </c>
+      <c r="B9" s="63" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="63" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="63"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="64">
+        <v>9</v>
+      </c>
+      <c r="B10" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="64" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="64" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="63">
+        <v>10</v>
+      </c>
+      <c r="B11" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="77"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="77">
-        <v>6</v>
-      </c>
-      <c r="B7" s="77" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="77" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7" s="77"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="77">
-        <v>7</v>
-      </c>
-      <c r="B8" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="77">
-        <v>8</v>
-      </c>
-      <c r="B9" s="77" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" s="77" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="77"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="78">
-        <v>9</v>
-      </c>
-      <c r="B10" s="78" t="s">
-        <v>107</v>
-      </c>
-      <c r="C10" s="78" t="s">
-        <v>108</v>
-      </c>
-      <c r="D10" s="78" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="77">
-        <v>10</v>
-      </c>
-      <c r="B11" s="77" t="s">
+      <c r="C11" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="77" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11" s="77"/>
+      <c r="D11" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Lagt till start och end date i add och edit
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19365" windowHeight="7155" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="114">
   <si>
     <t>Snabb översikt över produktionen</t>
   </si>
@@ -343,9 +343,6 @@
     <t>Se till att all css och responsibilitet fungerar på alla browsers</t>
   </si>
   <si>
-    <t>Ongoing</t>
-  </si>
-  <si>
     <t>Ändra ta bort todo $index till id istället</t>
   </si>
   <si>
@@ -365,6 +362,12 @@
   </si>
   <si>
     <t>Att admin knapparna syns när man är inne på admin sidorna.  Kolla Angular UI bootrstap.</t>
+  </si>
+  <si>
+    <t>Fixa så att de nuvarande datumen syns</t>
+  </si>
+  <si>
+    <t>På edit, add och fälten deadline, startdate och enddata</t>
   </si>
 </sst>
 </file>
@@ -414,7 +417,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -544,6 +547,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -713,7 +728,7 @@
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
@@ -779,6 +794,8 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="15" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="11" xfId="17" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="11" xfId="11" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="11" xfId="11" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="11" xfId="17" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="20% - Dekorfärg1" xfId="12" builtinId="30"/>
@@ -1223,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1577,7 +1594,7 @@
       </c>
       <c r="D21" s="41"/>
       <c r="E21" s="55" t="s">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="F21" s="29"/>
     </row>
@@ -1647,7 +1664,7 @@
       </c>
       <c r="D25" s="49"/>
       <c r="E25" s="42" t="s">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="F25" s="30" t="s">
         <v>92</v>
@@ -1935,10 +1952,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1983,7 +2000,7 @@
         <v>53</v>
       </c>
       <c r="D3" s="64" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2018,7 +2035,7 @@
         <v>100</v>
       </c>
       <c r="C6" s="63" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D6" s="63"/>
     </row>
@@ -2030,19 +2047,21 @@
         <v>101</v>
       </c>
       <c r="C7" s="63" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D7" s="63"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="63">
+      <c r="A8" s="66">
         <v>7</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="63">
@@ -2061,26 +2080,38 @@
         <v>9</v>
       </c>
       <c r="B10" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="D10" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="D10" s="64" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="63">
+      <c r="A11" s="65">
+        <v>11</v>
+      </c>
+      <c r="B11" s="65" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="65" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="65"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="63">
         <v>10</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B12" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="63" t="s">
-        <v>111</v>
-      </c>
-      <c r="D11" s="63"/>
+      <c r="D12" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Assignment controller plus tags
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maja\Documents\GitHub\ProjectPetra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Desktop\ProjectPetra\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1293,7 +1293,7 @@
   <dimension ref="A2:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1768,7 +1768,7 @@
       </c>
       <c r="D28" s="68"/>
       <c r="E28" s="68" t="s">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="F28" s="69" t="s">
         <v>118</v>

</xml_diff>

<commit_message>
Uppdaterat backlog och åtgärder
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Desktop\ProjectPetra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maja\Desktop\ProjectPetra\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="127">
   <si>
     <t>Snabb översikt över produktionen</t>
   </si>
@@ -456,7 +456,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="27">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -586,18 +586,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -772,9 +760,9 @@
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
@@ -840,11 +828,8 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="15" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="11" xfId="17" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="11" xfId="11" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="11" xfId="11" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="11" xfId="17" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="8" xfId="18" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="6" xfId="18" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="8" xfId="18" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="6" xfId="18" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="3" applyBorder="1"/>
   </cellXfs>
@@ -1293,7 +1278,7 @@
   <dimension ref="A2:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1723,90 +1708,90 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="70">
+      <c r="A26" s="67">
         <v>8</v>
       </c>
-      <c r="B26" s="70" t="s">
+      <c r="B26" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="C26" s="70">
+      <c r="C26" s="67">
         <v>46</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70" t="s">
+      <c r="D26" s="67"/>
+      <c r="E26" s="67" t="s">
         <v>125</v>
       </c>
-      <c r="F26" s="71"/>
+      <c r="F26" s="68"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="68" t="s">
+      <c r="A27" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="B27" s="68" t="s">
+      <c r="B27" s="65" t="s">
         <v>117</v>
       </c>
-      <c r="C27" s="68">
+      <c r="C27" s="65">
         <v>10</v>
       </c>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68" t="s">
+      <c r="D27" s="65"/>
+      <c r="E27" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="66" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="65" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="65">
+        <v>4</v>
+      </c>
+      <c r="D28" s="65"/>
+      <c r="E28" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="66" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="65">
+        <v>16</v>
+      </c>
+      <c r="D29" s="65"/>
+      <c r="E29" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="66" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="65">
+        <v>16</v>
+      </c>
+      <c r="D30" s="65"/>
+      <c r="E30" s="65" t="s">
         <v>125</v>
       </c>
-      <c r="F27" s="69" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="68" t="s">
-        <v>87</v>
-      </c>
-      <c r="B28" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="68">
-        <v>4</v>
-      </c>
-      <c r="D28" s="68"/>
-      <c r="E28" s="68" t="s">
-        <v>125</v>
-      </c>
-      <c r="F28" s="69" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="B29" s="68" t="s">
-        <v>70</v>
-      </c>
-      <c r="C29" s="68">
-        <v>16</v>
-      </c>
-      <c r="D29" s="68"/>
-      <c r="E29" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29" s="69" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="68" t="s">
-        <v>89</v>
-      </c>
-      <c r="B30" s="68" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="68">
-        <v>16</v>
-      </c>
-      <c r="D30" s="68"/>
-      <c r="E30" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" s="69" t="s">
+      <c r="F30" s="66" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2095,7 +2080,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,14 +2177,14 @@
       <c r="D7" s="63"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="66">
+      <c r="A8" s="64">
         <v>7</v>
       </c>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66" t="s">
+      <c r="C8" s="64"/>
+      <c r="D8" s="64" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2230,16 +2215,18 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="65">
+      <c r="A11" s="64">
         <v>11</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="65"/>
+      <c r="D11" s="64" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="63">
@@ -2254,16 +2241,16 @@
       <c r="D12" s="63"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="67">
+      <c r="A13" s="63">
         <v>12</v>
       </c>
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="D13" s="67"/>
+      <c r="D13" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>